<commit_message>
change to arg version
</commit_message>
<xml_diff>
--- a/ml_balanced_test.xlsx
+++ b/ml_balanced_test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ANA/McGill/Thesis_MER_Lyrics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ANA/McGill/Thesis_MER_Lyrics/Extract-Lyrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9530E8-9F71-A242-A474-E20C50D8DAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64C30B2-B3DE-1D4B-B393-11D05FE0311C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34560" yWindow="-80" windowWidth="24340" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>angry</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Unconditional Love</t>
   </si>
   <si>
-    <t>Kool &amp; The Gang</t>
-  </si>
-  <si>
     <t>Artist</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
   </si>
   <si>
     <t>Where'd All The Time Go?</t>
-  </si>
-  <si>
-    <t>Steppin' Into Love</t>
   </si>
 </sst>
 </file>
@@ -953,7 +947,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:D71"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -965,22 +959,22 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -988,10 +982,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -1011,10 +1005,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -1022,7 +1016,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1032,15 +1026,6 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>